<commit_message>
[IMP] change xlsx format
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
@@ -88,21 +88,15 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -125,21 +119,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +445,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -448,7 +473,7 @@
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -464,77 +489,77 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
[IMP] purchase summarize report condition
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>NSTDA</t>
   </si>
@@ -72,10 +72,6 @@
   </si>
   <si>
     <t>วันที่เอกสาร (Date Po)</t>
-  </si>
-  <si>
-    <t>ถ้า C&gt;100000=C
-ถ้า C&lt;=100000= ว่าง</t>
   </si>
   <si>
     <t>งานที่จัดซื้อหรือจัดจ้าง</t>
@@ -87,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -235,11 +231,11 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,58 +519,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" style="14" customWidth="1"/>
-    <col min="5" max="6" width="21.36328125" style="2"/>
-    <col min="7" max="7" width="21.36328125" style="14"/>
-    <col min="8" max="8" width="21.36328125" style="2"/>
-    <col min="9" max="9" width="21.36328125" style="14"/>
-    <col min="10" max="11" width="21.36328125" style="2"/>
-    <col min="12" max="12" width="21.36328125" style="18"/>
-    <col min="13" max="16384" width="21.36328125" style="3"/>
+    <col min="1" max="1" width="10.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="14" customWidth="1"/>
+    <col min="5" max="6" width="21.33203125" style="2"/>
+    <col min="7" max="7" width="21.33203125" style="14"/>
+    <col min="8" max="8" width="21.33203125" style="2"/>
+    <col min="9" max="9" width="21.33203125" style="14"/>
+    <col min="10" max="11" width="21.33203125" style="2"/>
+    <col min="12" max="12" width="21.33203125" style="17"/>
+    <col min="13" max="16384" width="21.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-    </row>
-    <row r="3" spans="1:12" ht="25" x14ac:dyDescent="0.25">
+      <c r="B2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="10" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:12" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -583,7 +577,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>7</v>
@@ -607,7 +601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="7"/>
       <c r="B6" s="12"/>
       <c r="C6" s="15"/>
@@ -618,7 +612,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="7"/>
       <c r="B7" s="13"/>
       <c r="C7" s="16"/>
@@ -629,7 +623,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>
       <c r="B8" s="13"/>
       <c r="C8" s="16"/>
@@ -640,7 +634,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="16"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="7"/>
       <c r="B9" s="13"/>
       <c r="C9" s="16"/>

</xml_diff>

<commit_message>
[ENH] rework on purchase summarize report
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -222,9 +222,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -237,12 +234,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -267,9 +258,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -294,11 +282,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,268 +574,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.08984375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" style="7" customWidth="1"/>
-    <col min="6" max="7" width="21.36328125" style="1"/>
-    <col min="8" max="8" width="21.36328125" style="7"/>
-    <col min="9" max="9" width="21.36328125" style="1"/>
-    <col min="10" max="10" width="21.36328125" style="7"/>
-    <col min="11" max="11" width="21.36328125" style="1"/>
+    <col min="1" max="1" width="16.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="6" customWidth="1"/>
+    <col min="6" max="7" width="21.33203125" style="1"/>
+    <col min="8" max="8" width="21.33203125" style="6"/>
+    <col min="9" max="9" width="21.33203125" style="1"/>
+    <col min="10" max="10" width="21.33203125" style="6"/>
+    <col min="11" max="11" width="21.33203125" style="1"/>
     <col min="12" max="12" width="25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.36328125" style="10"/>
-    <col min="14" max="16384" width="21.36328125" style="2"/>
+    <col min="13" max="13" width="21.33203125" style="7"/>
+    <col min="14" max="16384" width="21.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:13" s="11" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="1:13" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="9"/>
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="M12" s="26"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="M14" s="26"/>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M15" s="26"/>
+    </row>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M16" s="26"/>
+    </row>
+    <row r="17" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M19" s="26"/>
+    </row>
+    <row r="20" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M21" s="26"/>
+    </row>
+    <row r="22" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M22" s="26"/>
+    </row>
+    <row r="23" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M23" s="26"/>
+    </row>
+    <row r="24" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M24" s="26"/>
+    </row>
+    <row r="25" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M25" s="26"/>
+    </row>
+    <row r="26" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M26" s="26"/>
+    </row>
+    <row r="27" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M27" s="26"/>
+    </row>
+    <row r="28" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M28" s="26"/>
+    </row>
+    <row r="29" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M29" s="26"/>
+    </row>
+    <row r="30" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M30" s="26"/>
+    </row>
+    <row r="31" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M31" s="26"/>
+    </row>
+    <row r="32" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M32" s="26"/>
+    </row>
+    <row r="33" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M33" s="26"/>
+    </row>
+    <row r="34" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M34" s="26"/>
+    </row>
+    <row r="35" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M35" s="26"/>
+    </row>
+    <row r="36" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M36" s="26"/>
+    </row>
+    <row r="37" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M37" s="26"/>
+    </row>
+    <row r="38" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M38" s="26"/>
+    </row>
+    <row r="39" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M39" s="26"/>
+    </row>
+    <row r="40" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M40" s="26"/>
+    </row>
+    <row r="41" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M41" s="26"/>
+    </row>
+    <row r="42" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M42" s="26"/>
+    </row>
+    <row r="43" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M43" s="26"/>
+    </row>
+    <row r="44" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M44" s="26"/>
+    </row>
+    <row r="45" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M45" s="26"/>
+    </row>
+    <row r="46" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M46" s="26"/>
+    </row>
+    <row r="47" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M47" s="26"/>
+    </row>
+    <row r="48" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M48" s="26"/>
+    </row>
+    <row r="49" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M49" s="26"/>
+    </row>
+    <row r="50" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M50" s="26"/>
+    </row>
+    <row r="51" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M51" s="26"/>
+    </row>
+    <row r="52" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M52" s="26"/>
+    </row>
+    <row r="53" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M53" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[FIX] purchase_summarize : Change template layout.
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ลำดับที่</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>วันที่เอกสาร</t>
+  </si>
+  <si>
+    <t>ผู้รับผิดชอบ</t>
+  </si>
+  <si>
+    <t>สถานะ</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -225,12 +231,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -285,14 +285,26 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -585,378 +597,384 @@
     <col min="1" max="1" width="16.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
     <col min="6" max="7" width="21.33203125" style="1"/>
-    <col min="8" max="8" width="21.33203125" style="6"/>
+    <col min="8" max="8" width="21.33203125" style="4"/>
     <col min="9" max="9" width="21.33203125" style="1"/>
-    <col min="10" max="10" width="21.33203125" style="6"/>
+    <col min="10" max="10" width="21.33203125" style="4"/>
     <col min="11" max="11" width="21.33203125" style="1"/>
     <col min="12" max="12" width="25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="7"/>
+    <col min="13" max="13" width="21.33203125" style="5"/>
     <col min="14" max="16384" width="21.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:15" s="9" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="16" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="10"/>
-    </row>
-    <row r="3" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="16" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="16" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="16" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="12"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" s="18" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="M11" s="26"/>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="M12" s="26"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="M13" s="26"/>
-    </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="M14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M16" s="26"/>
-    </row>
-    <row r="17" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M17" s="26"/>
-    </row>
-    <row r="18" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M18" s="26"/>
-    </row>
-    <row r="19" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M19" s="26"/>
-    </row>
-    <row r="20" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M20" s="26"/>
-    </row>
-    <row r="21" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M21" s="26"/>
+      <c r="N10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="13" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M18" s="27"/>
+    </row>
+    <row r="19" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M19" s="27"/>
+    </row>
+    <row r="20" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M20" s="27"/>
+    </row>
+    <row r="21" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M21" s="27"/>
     </row>
     <row r="22" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M22" s="26"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M23" s="26"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M24" s="26"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M25" s="26"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M26" s="26"/>
+      <c r="M26" s="22"/>
     </row>
     <row r="27" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M27" s="26"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M28" s="26"/>
+      <c r="M28" s="22"/>
     </row>
     <row r="29" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M29" s="26"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M30" s="26"/>
+      <c r="M30" s="22"/>
     </row>
     <row r="31" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M31" s="26"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M32" s="26"/>
+      <c r="M32" s="22"/>
     </row>
     <row r="33" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M33" s="26"/>
+      <c r="M33" s="22"/>
     </row>
     <row r="34" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M34" s="26"/>
+      <c r="M34" s="22"/>
     </row>
     <row r="35" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M35" s="26"/>
+      <c r="M35" s="22"/>
     </row>
     <row r="36" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M36" s="26"/>
+      <c r="M36" s="22"/>
     </row>
     <row r="37" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M37" s="26"/>
+      <c r="M37" s="22"/>
     </row>
     <row r="38" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M38" s="26"/>
+      <c r="M38" s="22"/>
     </row>
     <row r="39" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M39" s="26"/>
+      <c r="M39" s="22"/>
     </row>
     <row r="40" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M40" s="26"/>
+      <c r="M40" s="22"/>
     </row>
     <row r="41" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M41" s="26"/>
+      <c r="M41" s="22"/>
     </row>
     <row r="42" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M42" s="26"/>
+      <c r="M42" s="22"/>
     </row>
     <row r="43" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M43" s="26"/>
+      <c r="M43" s="22"/>
     </row>
     <row r="44" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M44" s="26"/>
+      <c r="M44" s="22"/>
     </row>
     <row r="45" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M45" s="26"/>
+      <c r="M45" s="22"/>
     </row>
     <row r="46" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M46" s="26"/>
+      <c r="M46" s="22"/>
     </row>
     <row r="47" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M47" s="26"/>
+      <c r="M47" s="22"/>
     </row>
     <row r="48" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M48" s="26"/>
+      <c r="M48" s="22"/>
     </row>
     <row r="49" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M49" s="26"/>
+      <c r="M49" s="22"/>
     </row>
     <row r="50" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M50" s="26"/>
+      <c r="M50" s="22"/>
     </row>
     <row r="51" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M51" s="26"/>
+      <c r="M51" s="22"/>
     </row>
     <row r="52" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M52" s="26"/>
+      <c r="M52" s="22"/>
     </row>
     <row r="53" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M53" s="26"/>
+      <c r="M53" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
#3199 - insert fields on purchase summarize report
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="3420" windowWidth="22480" windowHeight="10000" tabRatio="500"/>
+    <workbookView xWindow="4425" yWindow="3420" windowWidth="22485" windowHeight="10005" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="150001"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ลำดับที่</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>สถานะ</t>
+  </si>
+  <si>
+    <t>สาขา</t>
+  </si>
+  <si>
+    <t>เลขประจำตัวผู้เสียภาษี</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="187" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -234,7 +240,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -243,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -252,13 +258,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -270,7 +276,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -285,33 +291,61 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -586,47 +620,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
-    <col min="6" max="7" width="21.33203125" style="1"/>
-    <col min="8" max="8" width="21.33203125" style="4"/>
-    <col min="9" max="9" width="21.33203125" style="1"/>
-    <col min="10" max="10" width="21.33203125" style="4"/>
-    <col min="11" max="11" width="21.33203125" style="1"/>
-    <col min="12" max="12" width="25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="5"/>
-    <col min="14" max="16384" width="21.33203125" style="2"/>
+    <col min="1" max="1" width="16.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
+    <col min="6" max="9" width="21.28515625" style="1"/>
+    <col min="10" max="10" width="21.28515625" style="4"/>
+    <col min="11" max="11" width="21.28515625" style="1"/>
+    <col min="12" max="12" width="21.28515625" style="4"/>
+    <col min="13" max="13" width="21.28515625" style="1"/>
+    <col min="14" max="14" width="25" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" style="5"/>
+    <col min="16" max="16384" width="21.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="9" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:17" s="9" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L1" s="7"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -635,15 +671,17 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L2" s="7"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
@@ -652,15 +690,17 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="8"/>
-    </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L3" s="7"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
@@ -669,15 +709,17 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L4" s="7"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -686,15 +728,17 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -703,15 +747,17 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
@@ -720,15 +766,17 @@
       <c r="D7" s="11"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
@@ -737,30 +785,34 @@
       <c r="D8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="L8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="20"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:15" s="18" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L9" s="7"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" s="18" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
@@ -779,202 +831,216 @@
       <c r="F10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="J10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="K10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="L10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="M10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="N10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="O10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="P10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="17" t="s">
+      <c r="Q10" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="M11" s="27"/>
-    </row>
-    <row r="12" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="13" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="M14" s="27"/>
-    </row>
-    <row r="15" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M15" s="27"/>
-    </row>
-    <row r="16" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M16" s="27"/>
-    </row>
-    <row r="17" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M17" s="27"/>
-    </row>
-    <row r="18" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M18" s="27"/>
-    </row>
-    <row r="19" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M19" s="27"/>
-    </row>
-    <row r="20" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M20" s="27"/>
-    </row>
-    <row r="21" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M21" s="27"/>
-    </row>
-    <row r="22" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M22" s="22"/>
-    </row>
-    <row r="23" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M23" s="22"/>
-    </row>
-    <row r="24" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M24" s="22"/>
-    </row>
-    <row r="25" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M25" s="22"/>
-    </row>
-    <row r="26" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M26" s="22"/>
-    </row>
-    <row r="27" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M27" s="22"/>
-    </row>
-    <row r="28" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M28" s="22"/>
-    </row>
-    <row r="29" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M29" s="22"/>
-    </row>
-    <row r="30" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M30" s="22"/>
-    </row>
-    <row r="31" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M31" s="22"/>
-    </row>
-    <row r="32" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M32" s="22"/>
-    </row>
-    <row r="33" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M33" s="22"/>
-    </row>
-    <row r="34" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M34" s="22"/>
-    </row>
-    <row r="35" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M35" s="22"/>
-    </row>
-    <row r="36" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M36" s="22"/>
-    </row>
-    <row r="37" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M37" s="22"/>
-    </row>
-    <row r="38" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M38" s="22"/>
-    </row>
-    <row r="39" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M39" s="22"/>
-    </row>
-    <row r="40" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M40" s="22"/>
-    </row>
-    <row r="41" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M41" s="22"/>
-    </row>
-    <row r="42" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M42" s="22"/>
-    </row>
-    <row r="43" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M43" s="22"/>
-    </row>
-    <row r="44" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M44" s="22"/>
-    </row>
-    <row r="45" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M45" s="22"/>
-    </row>
-    <row r="46" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M46" s="22"/>
-    </row>
-    <row r="47" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M47" s="22"/>
-    </row>
-    <row r="48" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M48" s="22"/>
-    </row>
-    <row r="49" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M49" s="22"/>
-    </row>
-    <row r="50" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M50" s="22"/>
-    </row>
-    <row r="51" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M51" s="22"/>
-    </row>
-    <row r="52" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M52" s="22"/>
-    </row>
-    <row r="53" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M53" s="22"/>
+    <row r="11" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="O11" s="26"/>
+    </row>
+    <row r="12" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="O12" s="26"/>
+    </row>
+    <row r="13" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="O13" s="26"/>
+    </row>
+    <row r="14" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="O14" s="26"/>
+    </row>
+    <row r="15" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O15" s="26"/>
+    </row>
+    <row r="16" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O16" s="26"/>
+    </row>
+    <row r="17" spans="15:15" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O17" s="26"/>
+    </row>
+    <row r="18" spans="15:15" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O18" s="26"/>
+    </row>
+    <row r="19" spans="15:15" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O19" s="26"/>
+    </row>
+    <row r="20" spans="15:15" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O20" s="26"/>
+    </row>
+    <row r="21" spans="15:15" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O21" s="26"/>
+    </row>
+    <row r="22" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O22" s="22"/>
+    </row>
+    <row r="23" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O23" s="22"/>
+    </row>
+    <row r="24" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O24" s="22"/>
+    </row>
+    <row r="25" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O25" s="22"/>
+    </row>
+    <row r="26" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O26" s="22"/>
+    </row>
+    <row r="27" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O27" s="22"/>
+    </row>
+    <row r="28" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O28" s="22"/>
+    </row>
+    <row r="29" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O29" s="22"/>
+    </row>
+    <row r="30" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O30" s="22"/>
+    </row>
+    <row r="31" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O31" s="22"/>
+    </row>
+    <row r="32" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O32" s="22"/>
+    </row>
+    <row r="33" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O33" s="22"/>
+    </row>
+    <row r="34" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O34" s="22"/>
+    </row>
+    <row r="35" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O35" s="22"/>
+    </row>
+    <row r="36" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O36" s="22"/>
+    </row>
+    <row r="37" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O37" s="22"/>
+    </row>
+    <row r="38" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O38" s="22"/>
+    </row>
+    <row r="39" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O39" s="22"/>
+    </row>
+    <row r="40" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O40" s="22"/>
+    </row>
+    <row r="41" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O41" s="22"/>
+    </row>
+    <row r="42" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O42" s="22"/>
+    </row>
+    <row r="43" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O43" s="22"/>
+    </row>
+    <row r="44" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O44" s="22"/>
+    </row>
+    <row r="45" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O45" s="22"/>
+    </row>
+    <row r="46" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O46" s="22"/>
+    </row>
+    <row r="47" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O47" s="22"/>
+    </row>
+    <row r="48" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O48" s="22"/>
+    </row>
+    <row r="49" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O49" s="22"/>
+    </row>
+    <row r="50" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O50" s="22"/>
+    </row>
+    <row r="51" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O51" s="22"/>
+    </row>
+    <row r="52" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O52" s="22"/>
+    </row>
+    <row r="53" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O53" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
#3199 - #3265 - edit Purchase Summarize and Supplier Evaluation report
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_summarize.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\DB\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="3420" windowWidth="22480" windowHeight="10000" tabRatio="500"/>
+    <workbookView xWindow="4425" yWindow="3420" windowWidth="22485" windowHeight="10005" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ลำดับที่</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>สถานะ</t>
+  </si>
+  <si>
+    <t>สาขา</t>
+  </si>
+  <si>
+    <t>เลขประจำตัวผู้เสียภาษี</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="187" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -234,7 +240,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -243,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -252,13 +258,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -270,7 +276,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -285,7 +291,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -300,7 +306,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -310,8 +316,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -586,30 +620,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
-    <col min="6" max="7" width="21.33203125" style="1"/>
-    <col min="8" max="8" width="21.33203125" style="4"/>
-    <col min="9" max="9" width="21.33203125" style="1"/>
-    <col min="10" max="10" width="21.33203125" style="4"/>
-    <col min="11" max="11" width="21.33203125" style="1"/>
-    <col min="12" max="12" width="25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="5"/>
-    <col min="14" max="16384" width="21.33203125" style="2"/>
+    <col min="1" max="1" width="16.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
+    <col min="6" max="9" width="21.28515625" style="1"/>
+    <col min="10" max="10" width="21.28515625" style="4"/>
+    <col min="11" max="11" width="21.28515625" style="1"/>
+    <col min="12" max="12" width="21.28515625" style="4"/>
+    <col min="13" max="13" width="21.28515625" style="1"/>
+    <col min="14" max="14" width="25" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" style="5"/>
+    <col min="16" max="16384" width="21.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="9" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" s="9" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
@@ -618,15 +652,17 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L1" s="7"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
@@ -635,15 +671,17 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L2" s="7"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
@@ -652,15 +690,17 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="8"/>
-    </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L3" s="7"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>12</v>
       </c>
@@ -669,15 +709,17 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L4" s="7"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -686,15 +728,17 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -703,15 +747,17 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
@@ -720,15 +766,17 @@
       <c r="D7" s="11"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:15" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
@@ -737,30 +785,34 @@
       <c r="D8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="L8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="20"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:15" s="18" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L9" s="7"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" s="18" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
@@ -779,35 +831,41 @@
       <c r="F10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="J10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="K10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="L10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="M10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="N10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="O10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="P10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="17" t="s">
+      <c r="Q10" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
@@ -818,9 +876,11 @@
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
-      <c r="M11" s="27"/>
-    </row>
-    <row r="12" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="O11" s="27"/>
+    </row>
+    <row r="12" spans="1:17" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
       <c r="C12" s="28"/>
@@ -831,9 +891,11 @@
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="13" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="O12" s="27"/>
+    </row>
+    <row r="13" spans="1:17" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24"/>
       <c r="B13" s="24"/>
       <c r="C13" s="28"/>
@@ -844,9 +906,11 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="O13" s="27"/>
+    </row>
+    <row r="14" spans="1:17" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="28"/>
@@ -857,124 +921,126 @@
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
-      <c r="M14" s="27"/>
-    </row>
-    <row r="15" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M15" s="27"/>
-    </row>
-    <row r="16" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M16" s="27"/>
-    </row>
-    <row r="17" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M17" s="27"/>
-    </row>
-    <row r="18" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M18" s="27"/>
-    </row>
-    <row r="19" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M19" s="27"/>
-    </row>
-    <row r="20" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M20" s="27"/>
-    </row>
-    <row r="21" spans="13:13" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M21" s="27"/>
-    </row>
-    <row r="22" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M22" s="22"/>
-    </row>
-    <row r="23" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M23" s="22"/>
-    </row>
-    <row r="24" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M24" s="22"/>
-    </row>
-    <row r="25" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M25" s="22"/>
-    </row>
-    <row r="26" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M26" s="22"/>
-    </row>
-    <row r="27" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M27" s="22"/>
-    </row>
-    <row r="28" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M28" s="22"/>
-    </row>
-    <row r="29" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M29" s="22"/>
-    </row>
-    <row r="30" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M30" s="22"/>
-    </row>
-    <row r="31" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M31" s="22"/>
-    </row>
-    <row r="32" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M32" s="22"/>
-    </row>
-    <row r="33" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M33" s="22"/>
-    </row>
-    <row r="34" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M34" s="22"/>
-    </row>
-    <row r="35" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M35" s="22"/>
-    </row>
-    <row r="36" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M36" s="22"/>
-    </row>
-    <row r="37" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M37" s="22"/>
-    </row>
-    <row r="38" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M38" s="22"/>
-    </row>
-    <row r="39" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M39" s="22"/>
-    </row>
-    <row r="40" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M40" s="22"/>
-    </row>
-    <row r="41" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M41" s="22"/>
-    </row>
-    <row r="42" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M42" s="22"/>
-    </row>
-    <row r="43" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M43" s="22"/>
-    </row>
-    <row r="44" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M44" s="22"/>
-    </row>
-    <row r="45" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M45" s="22"/>
-    </row>
-    <row r="46" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M46" s="22"/>
-    </row>
-    <row r="47" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M47" s="22"/>
-    </row>
-    <row r="48" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M48" s="22"/>
-    </row>
-    <row r="49" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M49" s="22"/>
-    </row>
-    <row r="50" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M50" s="22"/>
-    </row>
-    <row r="51" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M51" s="22"/>
-    </row>
-    <row r="52" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M52" s="22"/>
-    </row>
-    <row r="53" spans="13:13" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="M53" s="22"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="O14" s="27"/>
+    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O15" s="22"/>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O16" s="22"/>
+    </row>
+    <row r="17" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O17" s="22"/>
+    </row>
+    <row r="18" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O18" s="22"/>
+    </row>
+    <row r="19" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O19" s="22"/>
+    </row>
+    <row r="20" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O20" s="22"/>
+    </row>
+    <row r="21" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O21" s="22"/>
+    </row>
+    <row r="22" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O22" s="22"/>
+    </row>
+    <row r="23" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O23" s="22"/>
+    </row>
+    <row r="24" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O24" s="22"/>
+    </row>
+    <row r="25" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O25" s="22"/>
+    </row>
+    <row r="26" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O26" s="22"/>
+    </row>
+    <row r="27" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O27" s="22"/>
+    </row>
+    <row r="28" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O28" s="22"/>
+    </row>
+    <row r="29" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O29" s="22"/>
+    </row>
+    <row r="30" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O30" s="22"/>
+    </row>
+    <row r="31" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O31" s="22"/>
+    </row>
+    <row r="32" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O32" s="22"/>
+    </row>
+    <row r="33" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O33" s="22"/>
+    </row>
+    <row r="34" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O34" s="22"/>
+    </row>
+    <row r="35" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O35" s="22"/>
+    </row>
+    <row r="36" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O36" s="22"/>
+    </row>
+    <row r="37" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O37" s="22"/>
+    </row>
+    <row r="38" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O38" s="22"/>
+    </row>
+    <row r="39" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O39" s="22"/>
+    </row>
+    <row r="40" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O40" s="22"/>
+    </row>
+    <row r="41" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O41" s="22"/>
+    </row>
+    <row r="42" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O42" s="22"/>
+    </row>
+    <row r="43" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O43" s="22"/>
+    </row>
+    <row r="44" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O44" s="22"/>
+    </row>
+    <row r="45" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O45" s="22"/>
+    </row>
+    <row r="46" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O46" s="22"/>
+    </row>
+    <row r="47" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O47" s="22"/>
+    </row>
+    <row r="48" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O48" s="22"/>
+    </row>
+    <row r="49" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O49" s="22"/>
+    </row>
+    <row r="50" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O50" s="22"/>
+    </row>
+    <row r="51" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O51" s="22"/>
+    </row>
+    <row r="52" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O52" s="22"/>
+    </row>
+    <row r="53" spans="15:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O53" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>